<commit_message>
Use inmemory H2 DB instead of postgres
</commit_message>
<xml_diff>
--- a/NNSU_DB.xlsx
+++ b/NNSU_DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="1" r:id="rId1"/>
@@ -665,7 +665,7 @@
     <tableColumn id="1" name="full_address"/>
     <tableColumn id="2" name="id"/>
     <tableColumn id="3" name="SQL" dataDxfId="3">
-      <calculatedColumnFormula>"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</calculatedColumnFormula>
+      <calculatedColumnFormula>"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -679,7 +679,7 @@
     <tableColumn id="1" name="name"/>
     <tableColumn id="2" name="id"/>
     <tableColumn id="3" name="SQL" dataDxfId="2">
-      <calculatedColumnFormula>"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;CustomerStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</calculatedColumnFormula>
+      <calculatedColumnFormula>"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;CustomerStatusTable[[#This Row],[name]]&amp;"');"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -693,7 +693,7 @@
     <tableColumn id="1" name="name"/>
     <tableColumn id="2" name="id"/>
     <tableColumn id="3" name="SQL" dataDxfId="1">
-      <calculatedColumnFormula>"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;ServiceStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</calculatedColumnFormula>
+      <calculatedColumnFormula>"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;ServiceStatusTable[[#This Row],[name]]&amp;"');"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -707,7 +707,7 @@
     <tableColumn id="1" name="name"/>
     <tableColumn id="2" name="id"/>
     <tableColumn id="3" name="SQL" dataDxfId="0">
-      <calculatedColumnFormula>"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;HardwareStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</calculatedColumnFormula>
+      <calculatedColumnFormula>"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;HardwareStatusTable[[#This Row],[name]]&amp;"');"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -994,8 +994,8 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,8 +1506,8 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,7 +2380,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,8 +2409,8 @@
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул ломоносова д 23') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул ломоносова д 23');</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2421,8 +2421,8 @@
         <v>2</v>
       </c>
       <c r="C3" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A2),FIND("]",CELL("filename",A2))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул северная  д 30') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A2),FIND("]",CELL("filename",A2))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул северная  д 30');</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2433,8 +2433,8 @@
         <v>3</v>
       </c>
       <c r="C4" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A3),FIND("]",CELL("filename",A3))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 1') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A3),FIND("]",CELL("filename",A3))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 1');</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2445,8 +2445,8 @@
         <v>4</v>
       </c>
       <c r="C5" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A4),FIND("]",CELL("filename",A4))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 2') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A4),FIND("]",CELL("filename",A4))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 2');</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2457,8 +2457,8 @@
         <v>5</v>
       </c>
       <c r="C6" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A5),FIND("]",CELL("filename",A5))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 3') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A5),FIND("]",CELL("filename",A5))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 3');</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2469,8 +2469,8 @@
         <v>6</v>
       </c>
       <c r="C7" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A6),FIND("]",CELL("filename",A6))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 4') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A6),FIND("]",CELL("filename",A6))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 4');</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2481,8 +2481,8 @@
         <v>7</v>
       </c>
       <c r="C8" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A7),FIND("]",CELL("filename",A7))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 5') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A7),FIND("]",CELL("filename",A7))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 5');</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2493,8 +2493,8 @@
         <v>8</v>
       </c>
       <c r="C9" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A8),FIND("]",CELL("filename",A8))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 6') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A8),FIND("]",CELL("filename",A8))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул рождественская д 6');</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2505,8 +2505,8 @@
         <v>9</v>
       </c>
       <c r="C10" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A9),FIND("]",CELL("filename",A9))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 1') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A9),FIND("]",CELL("filename",A9))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 1');</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2517,8 +2517,8 @@
         <v>10</v>
       </c>
       <c r="C11" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A10),FIND("]",CELL("filename",A10))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 2') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A10),FIND("]",CELL("filename",A10))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 2');</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2529,8 +2529,8 @@
         <v>11</v>
       </c>
       <c r="C12" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A11),FIND("]",CELL("filename",A11))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 3') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A11),FIND("]",CELL("filename",A11))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 3');</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2541,8 +2541,8 @@
         <v>12</v>
       </c>
       <c r="C13" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A12),FIND("]",CELL("filename",A12))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 4') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A12),FIND("]",CELL("filename",A12))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 4');</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2553,8 +2553,8 @@
         <v>13</v>
       </c>
       <c r="C14" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A13),FIND("]",CELL("filename",A13))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 5') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A13),FIND("]",CELL("filename",A13))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 5');</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2565,8 +2565,8 @@
         <v>14</v>
       </c>
       <c r="C15" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A14),FIND("]",CELL("filename",A14))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 6') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A14),FIND("]",CELL("filename",A14))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул выборгская д 6');</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2577,8 +2577,8 @@
         <v>15</v>
       </c>
       <c r="C16" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A15),FIND("]",CELL("filename",A15))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 1') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A15),FIND("]",CELL("filename",A15))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 1');</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2589,8 +2589,8 @@
         <v>16</v>
       </c>
       <c r="C17" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A16),FIND("]",CELL("filename",A16))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 2') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A16),FIND("]",CELL("filename",A16))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 2');</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2601,8 +2601,8 @@
         <v>17</v>
       </c>
       <c r="C18" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A17),FIND("]",CELL("filename",A17))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 3') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A17),FIND("]",CELL("filename",A17))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 3');</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2613,8 +2613,8 @@
         <v>18</v>
       </c>
       <c r="C19" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A18),FIND("]",CELL("filename",A18))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 4') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A18),FIND("]",CELL("filename",A18))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 4');</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2625,8 +2625,8 @@
         <v>19</v>
       </c>
       <c r="C20" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A19),FIND("]",CELL("filename",A19))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 5') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A19),FIND("]",CELL("filename",A19))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 5');</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2637,8 +2637,8 @@
         <v>20</v>
       </c>
       <c r="C21" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A20),FIND("]",CELL("filename",A20))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 6') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A20),FIND("]",CELL("filename",A20))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул гужевая д 6');</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2649,8 +2649,8 @@
         <v>21</v>
       </c>
       <c r="C22" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A21),FIND("]",CELL("filename",A21))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул минина д 1') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A21),FIND("]",CELL("filename",A21))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул минина д 1');</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2661,8 +2661,8 @@
         <v>22</v>
       </c>
       <c r="C23" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A22),FIND("]",CELL("filename",A22))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул минина д 2') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A22),FIND("]",CELL("filename",A22))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул минина д 2');</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2673,8 +2673,8 @@
         <v>23</v>
       </c>
       <c r="C24" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A23),FIND("]",CELL("filename",A23))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;"</f>
-        <v>INSERT INTO address (full_address) VALUES ('ул минина д 3') ON CONFLICT (full_address) DO UPDATE SET full_address=EXCLUDED.full_address;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A23),FIND("]",CELL("filename",A23))+1,255)&amp;" (full_address) VALUES ('"&amp;AddressTable[[#This Row],[full_address]]&amp;"');"</f>
+        <v>INSERT INTO address (full_address) VALUES ('ул минина д 3');</v>
       </c>
     </row>
   </sheetData>
@@ -2693,7 +2693,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2720,8 +2720,8 @@
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;CustomerStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</f>
-        <v>INSERT INTO customer_status (name) VALUES ('NORMAL') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;CustomerStatusTable[[#This Row],[name]]&amp;"');"</f>
+        <v>INSERT INTO customer_status (name) VALUES ('NORMAL');</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2732,8 +2732,8 @@
         <v>2</v>
       </c>
       <c r="C3" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A2),FIND("]",CELL("filename",A2))+1,255)&amp;" (name) VALUES ('"&amp;CustomerStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</f>
-        <v>INSERT INTO customer_status (name) VALUES ('FAIL') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A2),FIND("]",CELL("filename",A2))+1,255)&amp;" (name) VALUES ('"&amp;CustomerStatusTable[[#This Row],[name]]&amp;"');"</f>
+        <v>INSERT INTO customer_status (name) VALUES ('FAIL');</v>
       </c>
     </row>
   </sheetData>
@@ -2752,7 +2752,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2780,8 +2780,8 @@
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;ServiceStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</f>
-        <v>INSERT INTO service_status (name) VALUES ('NORMAL') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;ServiceStatusTable[[#This Row],[name]]&amp;"');"</f>
+        <v>INSERT INTO service_status (name) VALUES ('NORMAL');</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2792,8 +2792,8 @@
         <v>2</v>
       </c>
       <c r="C3" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A2),FIND("]",CELL("filename",A2))+1,255)&amp;" (name) VALUES ('"&amp;ServiceStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</f>
-        <v>INSERT INTO service_status (name) VALUES ('FAIL') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A2),FIND("]",CELL("filename",A2))+1,255)&amp;" (name) VALUES ('"&amp;ServiceStatusTable[[#This Row],[name]]&amp;"');"</f>
+        <v>INSERT INTO service_status (name) VALUES ('FAIL');</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2804,8 +2804,8 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A3),FIND("]",CELL("filename",A3))+1,255)&amp;" (name) VALUES ('"&amp;ServiceStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</f>
-        <v>INSERT INTO service_status (name) VALUES ('UNDER_MAINT') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A3),FIND("]",CELL("filename",A3))+1,255)&amp;" (name) VALUES ('"&amp;ServiceStatusTable[[#This Row],[name]]&amp;"');"</f>
+        <v>INSERT INTO service_status (name) VALUES ('UNDER_MAINT');</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2816,8 +2816,8 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A4),FIND("]",CELL("filename",A4))+1,255)&amp;" (name) VALUES ('"&amp;ServiceStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</f>
-        <v>INSERT INTO service_status (name) VALUES ('TO_REPLACE') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A4),FIND("]",CELL("filename",A4))+1,255)&amp;" (name) VALUES ('"&amp;ServiceStatusTable[[#This Row],[name]]&amp;"');"</f>
+        <v>INSERT INTO service_status (name) VALUES ('TO_REPLACE');</v>
       </c>
     </row>
   </sheetData>
@@ -2837,7 +2837,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,8 +2865,8 @@
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;HardwareStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</f>
-        <v>INSERT INTO hardware_status (name) VALUES ('NORMAL') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" (name) VALUES ('"&amp;HardwareStatusTable[[#This Row],[name]]&amp;"');"</f>
+        <v>INSERT INTO hardware_status (name) VALUES ('NORMAL');</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2877,8 +2877,8 @@
         <v>2</v>
       </c>
       <c r="C3" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A2),FIND("]",CELL("filename",A2))+1,255)&amp;" (name) VALUES ('"&amp;HardwareStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</f>
-        <v>INSERT INTO hardware_status (name) VALUES ('FAIL') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A2),FIND("]",CELL("filename",A2))+1,255)&amp;" (name) VALUES ('"&amp;HardwareStatusTable[[#This Row],[name]]&amp;"');"</f>
+        <v>INSERT INTO hardware_status (name) VALUES ('FAIL');</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2889,8 +2889,8 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A3),FIND("]",CELL("filename",A3))+1,255)&amp;" (name) VALUES ('"&amp;HardwareStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</f>
-        <v>INSERT INTO hardware_status (name) VALUES ('UNDER_MAINT') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A3),FIND("]",CELL("filename",A3))+1,255)&amp;" (name) VALUES ('"&amp;HardwareStatusTable[[#This Row],[name]]&amp;"');"</f>
+        <v>INSERT INTO hardware_status (name) VALUES ('UNDER_MAINT');</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2901,8 +2901,8 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A4),FIND("]",CELL("filename",A4))+1,255)&amp;" (name) VALUES ('"&amp;HardwareStatusTable[[#This Row],[name]]&amp;"') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;"</f>
-        <v>INSERT INTO hardware_status (name) VALUES ('TO_REPLACE') ON CONFLICT (name) DO UPDATE SET name=EXCLUDED.name;</v>
+        <f ca="1">"INSERT INTO "&amp;MID(CELL("filename",A4),FIND("]",CELL("filename",A4))+1,255)&amp;" (name) VALUES ('"&amp;HardwareStatusTable[[#This Row],[name]]&amp;"');"</f>
+        <v>INSERT INTO hardware_status (name) VALUES ('TO_REPLACE');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>